<commit_message>
minor subgroups added in compulsory minor - works
</commit_message>
<xml_diff>
--- a/testData/Offered_Course_List_spring2019.xlsx
+++ b/testData/Offered_Course_List_spring2019.xlsx
@@ -4208,9 +4208,9 @@
   <dimension ref="A1:BZ280"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="H119" activeCellId="0" sqref="H119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
link to result added
</commit_message>
<xml_diff>
--- a/testData/Offered_Course_List_spring2019.xlsx
+++ b/testData/Offered_Course_List_spring2019.xlsx
@@ -953,26 +953,8 @@
 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ENG343TUT1instructor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
+    <t xml:space="preserve">ENG343TUT1instructor,
+</t>
   </si>
   <si>
     <t xml:space="preserve">Teja Varma Pusapati[20500842]</t>
@@ -988,26 +970,8 @@
 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ENG445TUT1instructor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
+    <t xml:space="preserve">ENG445TUT1instructor,
+</t>
   </si>
   <si>
     <t xml:space="preserve">Tulika  Chandra[20500029]</t>
@@ -1023,26 +987,8 @@
 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ENG444TUT1instructor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
+    <t xml:space="preserve">ENG444TUT1instructor,
+</t>
   </si>
   <si>
     <t xml:space="preserve">Vikram  Kapur[20500186]</t>
@@ -1084,26 +1030,8 @@
 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ENG344TUT1instructor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
+    <t xml:space="preserve">ENG344TUT1instructor,
+</t>
   </si>
   <si>
     <t xml:space="preserve">CCC629</t>
@@ -1415,26 +1343,8 @@
 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ENG142TUT1instructor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
+    <t xml:space="preserve">ENG142TUT1instructor,
+</t>
   </si>
   <si>
     <t xml:space="preserve">Aniket  Devendra Jaaware[20500860]</t>
@@ -1446,26 +1356,8 @@
     <t xml:space="preserve">Drama: Tropes and Adaptations</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ENG143TUT1instructor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
+    <t xml:space="preserve">ENG143TUT1instructor,
+</t>
   </si>
   <si>
     <t xml:space="preserve">EED308</t>
@@ -1967,70 +1859,16 @@
     <t xml:space="preserve">Economics1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ECO101Lec1Instrucotor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ECO101Tut1Instrucotor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ECO101Tut2Instrucotor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
+    <t xml:space="preserve">ECO101Lec1Instrucotor,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECO101Tut1Instrucotor,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECO101Tut2Instrucotor,
+</t>
   </si>
   <si>
     <t xml:space="preserve">ECO102</t>
@@ -2059,95 +1897,23 @@
     <t xml:space="preserve">Pre-requisite for this course is ECO101/MEC102</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ECO102TA2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ECO102TA3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ECO102TA4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
+    <t xml:space="preserve">ECO102TA2,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECO102TA3,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECO102TA4,
+</t>
   </si>
   <si>
     <t xml:space="preserve">TUT5</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ECO102TA5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
+    <t xml:space="preserve">ECO102TA5,
+</t>
   </si>
   <si>
     <t xml:space="preserve">ECO302</t>
@@ -2723,26 +2489,8 @@
 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ENG346Tut1Instrucotor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
+    <t xml:space="preserve">ENG346Tut1Instrucotor,
+</t>
   </si>
   <si>
     <t xml:space="preserve">Aakriti  Mandhwani[20500931]</t>
@@ -3349,114 +3097,24 @@
 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MAT104TA2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MAT104TA3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MAT104TA4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MAT104TA5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MAT104TA6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
+    <t xml:space="preserve">MAT104TA2,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAT104TA3,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAT104TA4,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAT104TA5,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAT104TA6,
+</t>
   </si>
   <si>
     <t xml:space="preserve">MAT084</t>
@@ -4253,26 +3911,8 @@
     <t xml:space="preserve">A Global History of Science</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">HIS313Lec1Insttructor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
+    <t xml:space="preserve">HIS313Lec1Insttructor,
+</t>
   </si>
   <si>
     <t xml:space="preserve">The course will be offered by Prof. Kapil Raj, who is a Visiting Professor.</t>
@@ -4329,26 +3969,8 @@
 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ENG104TA1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
+    <t xml:space="preserve">ENG104TA1,
+</t>
   </si>
   <si>
     <t xml:space="preserve">Anirban  Ghosh[20500908]</t>
@@ -4358,26 +3980,8 @@
 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ENG104TA2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,
-</t>
-    </r>
+    <t xml:space="preserve">ENG104TA2,
+</t>
   </si>
   <si>
     <t xml:space="preserve">INT142</t>
@@ -4485,7 +4089,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4515,12 +4119,6 @@
       <name val="Georgia"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4585,7 +4183,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -4606,7 +4204,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4614,7 +4212,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4622,11 +4220,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4718,10 +4316,10 @@
   </sheetPr>
   <dimension ref="A1:BZ280"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D103" activeCellId="0" sqref="D103"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="G102" activeCellId="0" sqref="G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4732,7 +4330,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="9" style="1" width="29.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="15.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="16.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="19.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="27" style="1" width="29.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="60" style="2" width="8.96"/>
@@ -22456,7 +22054,7 @@
   </sheetPr>
   <dimension ref="A1:C213"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
restricting options in UWE from 2 to 1, and CCC from all to 1 gives slightly more compact schedule
</commit_message>
<xml_diff>
--- a/testData/Offered_Course_List_spring2019.xlsx
+++ b/testData/Offered_Course_List_spring2019.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4414" uniqueCount="1156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4414" uniqueCount="1155">
   <si>
     <t xml:space="preserve">School</t>
   </si>
@@ -3893,9 +3893,6 @@
   </si>
   <si>
     <t xml:space="preserve">Agri-Food Systems:............</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Under Graduate1</t>
   </si>
   <si>
     <t xml:space="preserve">Rajeswari Sarala Raina[20500660],
@@ -4316,10 +4313,10 @@
   </sheetPr>
   <dimension ref="A1:BZ280"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="G102" activeCellId="0" sqref="G102"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A263" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="H266" activeCellId="0" sqref="H266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20867,7 +20864,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="266" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="266" customFormat="false" ht="42.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="s">
         <v>249</v>
       </c>
@@ -20893,7 +20890,7 @@
         <v>120</v>
       </c>
       <c r="I266" s="1" t="s">
-        <v>1101</v>
+        <v>1087</v>
       </c>
       <c r="S266" s="1" t="n">
         <v>25</v>
@@ -20914,19 +20911,19 @@
         <v>75</v>
       </c>
       <c r="AA266" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="AB266" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="AG266" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH266" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM266" s="1" t="s">
         <v>1102</v>
-      </c>
-      <c r="AB266" s="1" t="s">
-        <v>1102</v>
-      </c>
-      <c r="AG266" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH266" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM266" s="1" t="s">
-        <v>1103</v>
       </c>
       <c r="AN266" s="1" t="n">
         <v>3</v>
@@ -20955,10 +20952,10 @@
         <v>404</v>
       </c>
       <c r="C267" s="1" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D267" s="1" t="s">
         <v>1104</v>
-      </c>
-      <c r="D267" s="1" t="s">
-        <v>1105</v>
       </c>
       <c r="E267" s="1" t="n">
         <v>4</v>
@@ -20994,10 +20991,10 @@
         <v>75</v>
       </c>
       <c r="AA267" s="4" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="AB267" s="4" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="AF267" s="1" t="s">
         <v>409</v>
@@ -21009,10 +21006,10 @@
         <v>59</v>
       </c>
       <c r="AJ267" s="1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="AK267" s="1" t="s">
         <v>1107</v>
-      </c>
-      <c r="AK267" s="1" t="s">
-        <v>1108</v>
       </c>
       <c r="AM267" s="1" t="s">
         <v>281</v>
@@ -21027,7 +21024,7 @@
         <v>0</v>
       </c>
       <c r="AQ267" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="AT267" s="1" t="s">
         <v>59</v>
@@ -21044,10 +21041,10 @@
         <v>701</v>
       </c>
       <c r="C268" s="1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D268" s="1" t="s">
         <v>1110</v>
-      </c>
-      <c r="D268" s="1" t="s">
-        <v>1111</v>
       </c>
       <c r="E268" s="1" t="n">
         <v>3</v>
@@ -21080,10 +21077,10 @@
         <v>56</v>
       </c>
       <c r="AA268" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="AC268" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="AD268" s="1" t="s">
         <v>705</v>
@@ -21098,7 +21095,7 @@
         <v>59</v>
       </c>
       <c r="AM268" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="AN268" s="1" t="n">
         <v>1</v>
@@ -21110,7 +21107,7 @@
         <v>2</v>
       </c>
       <c r="AQ268" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="AT268" s="1" t="s">
         <v>59</v>
@@ -21127,10 +21124,10 @@
         <v>701</v>
       </c>
       <c r="C269" s="1" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D269" s="1" t="s">
         <v>1115</v>
-      </c>
-      <c r="D269" s="1" t="s">
-        <v>1116</v>
       </c>
       <c r="E269" s="1" t="n">
         <v>3</v>
@@ -21163,10 +21160,10 @@
         <v>56</v>
       </c>
       <c r="AA269" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="AC269" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="AD269" s="1" t="s">
         <v>705</v>
@@ -21181,7 +21178,7 @@
         <v>59</v>
       </c>
       <c r="AM269" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="AN269" s="1" t="n">
         <v>1</v>
@@ -21193,7 +21190,7 @@
         <v>2</v>
       </c>
       <c r="AQ269" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="AT269" s="1" t="s">
         <v>59</v>
@@ -21210,10 +21207,10 @@
         <v>250</v>
       </c>
       <c r="C270" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D270" s="1" t="s">
         <v>1118</v>
-      </c>
-      <c r="D270" s="1" t="s">
-        <v>1119</v>
       </c>
       <c r="E270" s="1" t="n">
         <v>4</v>
@@ -21246,10 +21243,10 @@
         <v>75</v>
       </c>
       <c r="AA270" s="1" t="s">
+        <v>1119</v>
+      </c>
+      <c r="AB270" s="4" t="s">
         <v>1120</v>
-      </c>
-      <c r="AB270" s="4" t="s">
-        <v>1121</v>
       </c>
       <c r="AG270" s="1" t="s">
         <v>52</v>
@@ -21258,19 +21255,19 @@
         <v>59</v>
       </c>
       <c r="AM270" s="1" t="s">
+        <v>1121</v>
+      </c>
+      <c r="AN270" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO270" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP270" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ270" s="1" t="s">
         <v>1122</v>
-      </c>
-      <c r="AN270" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="AO270" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP270" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ270" s="1" t="s">
-        <v>1123</v>
       </c>
       <c r="AT270" s="1" t="s">
         <v>59</v>
@@ -21287,10 +21284,10 @@
         <v>81</v>
       </c>
       <c r="AA271" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="AB271" s="4" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21301,10 +21298,10 @@
         <v>1084</v>
       </c>
       <c r="C272" s="1" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D272" s="1" t="s">
         <v>1125</v>
-      </c>
-      <c r="D272" s="1" t="s">
-        <v>1126</v>
       </c>
       <c r="E272" s="1" t="n">
         <v>4</v>
@@ -21337,19 +21334,19 @@
         <v>75</v>
       </c>
       <c r="AA272" s="1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="AB272" s="1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="AG272" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH272" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM272" s="1" t="s">
         <v>1127</v>
-      </c>
-      <c r="AB272" s="1" t="s">
-        <v>1127</v>
-      </c>
-      <c r="AG272" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH272" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM272" s="1" t="s">
-        <v>1128</v>
       </c>
       <c r="AN272" s="1" t="n">
         <v>3</v>
@@ -21378,10 +21375,10 @@
         <v>1084</v>
       </c>
       <c r="C273" s="1" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D273" s="1" t="s">
         <v>1129</v>
-      </c>
-      <c r="D273" s="1" t="s">
-        <v>1130</v>
       </c>
       <c r="E273" s="1" t="n">
         <v>4</v>
@@ -21414,19 +21411,19 @@
         <v>75</v>
       </c>
       <c r="AA273" s="1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="AB273" s="1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="AG273" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH273" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM273" s="1" t="s">
         <v>1127</v>
-      </c>
-      <c r="AB273" s="1" t="s">
-        <v>1127</v>
-      </c>
-      <c r="AG273" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH273" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM273" s="1" t="s">
-        <v>1128</v>
       </c>
       <c r="AN273" s="1" t="n">
         <v>3</v>
@@ -21455,10 +21452,10 @@
         <v>340</v>
       </c>
       <c r="C274" s="1" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D274" s="1" t="s">
         <v>1131</v>
-      </c>
-      <c r="D274" s="1" t="s">
-        <v>1132</v>
       </c>
       <c r="E274" s="1" t="n">
         <v>3</v>
@@ -21541,10 +21538,10 @@
         <v>340</v>
       </c>
       <c r="C275" s="1" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D275" s="1" t="s">
         <v>1133</v>
-      </c>
-      <c r="D275" s="1" t="s">
-        <v>1134</v>
       </c>
       <c r="E275" s="1" t="n">
         <v>3</v>
@@ -21586,7 +21583,7 @@
         <v>351</v>
       </c>
       <c r="AD275" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="AE275" s="1" t="n">
         <v>30</v>
@@ -21613,7 +21610,7 @@
         <v>80</v>
       </c>
       <c r="AS275" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="AT275" s="1" t="s">
         <v>59</v>
@@ -21630,7 +21627,7 @@
         <v>860</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D276" s="1" t="s">
         <v>361</v>
@@ -21713,10 +21710,10 @@
         <v>860</v>
       </c>
       <c r="C277" s="1" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D277" s="1" t="s">
         <v>1138</v>
-      </c>
-      <c r="D277" s="1" t="s">
-        <v>1139</v>
       </c>
       <c r="E277" s="1" t="n">
         <v>4</v>
@@ -21749,19 +21746,19 @@
         <v>75</v>
       </c>
       <c r="AA277" s="1" t="s">
+        <v>1139</v>
+      </c>
+      <c r="AB277" s="1" t="s">
+        <v>1139</v>
+      </c>
+      <c r="AG277" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH277" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM277" s="1" t="s">
         <v>1140</v>
-      </c>
-      <c r="AB277" s="1" t="s">
-        <v>1140</v>
-      </c>
-      <c r="AG277" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH277" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM277" s="1" t="s">
-        <v>1141</v>
       </c>
       <c r="AN277" s="1" t="n">
         <v>3</v>
@@ -21790,10 +21787,10 @@
         <v>860</v>
       </c>
       <c r="C278" s="1" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D278" s="1" t="s">
         <v>1142</v>
-      </c>
-      <c r="D278" s="1" t="s">
-        <v>1143</v>
       </c>
       <c r="E278" s="1" t="n">
         <v>4</v>
@@ -21832,22 +21829,22 @@
         <v>75</v>
       </c>
       <c r="AA278" s="1" t="s">
+        <v>1143</v>
+      </c>
+      <c r="AB278" s="1" t="s">
+        <v>1143</v>
+      </c>
+      <c r="AF278" s="1" t="s">
         <v>1144</v>
       </c>
-      <c r="AB278" s="1" t="s">
-        <v>1144</v>
-      </c>
-      <c r="AF278" s="1" t="s">
+      <c r="AG278" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH278" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM278" s="1" t="s">
         <v>1145</v>
-      </c>
-      <c r="AG278" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH278" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM278" s="1" t="s">
-        <v>1146</v>
       </c>
       <c r="AN278" s="1" t="n">
         <v>3</v>
@@ -21876,10 +21873,10 @@
         <v>860</v>
       </c>
       <c r="C279" s="1" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D279" s="1" t="s">
         <v>1147</v>
-      </c>
-      <c r="D279" s="1" t="s">
-        <v>1148</v>
       </c>
       <c r="E279" s="1" t="n">
         <v>4</v>
@@ -21915,19 +21912,19 @@
         <v>75</v>
       </c>
       <c r="AA279" s="1" t="s">
+        <v>1148</v>
+      </c>
+      <c r="AB279" s="1" t="s">
+        <v>1148</v>
+      </c>
+      <c r="AG279" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH279" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM279" s="1" t="s">
         <v>1149</v>
-      </c>
-      <c r="AB279" s="1" t="s">
-        <v>1149</v>
-      </c>
-      <c r="AG279" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH279" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM279" s="1" t="s">
-        <v>1150</v>
       </c>
       <c r="AN279" s="1" t="n">
         <v>3</v>
@@ -21942,7 +21939,7 @@
         <v>867</v>
       </c>
       <c r="AS279" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="AT279" s="1" t="s">
         <v>59</v>
@@ -21959,10 +21956,10 @@
         <v>860</v>
       </c>
       <c r="C280" s="1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D280" s="1" t="s">
         <v>1152</v>
-      </c>
-      <c r="D280" s="1" t="s">
-        <v>1153</v>
       </c>
       <c r="E280" s="1" t="n">
         <v>4</v>
@@ -22001,19 +21998,19 @@
         <v>75</v>
       </c>
       <c r="AA280" s="1" t="s">
+        <v>1153</v>
+      </c>
+      <c r="AB280" s="1" t="s">
+        <v>1153</v>
+      </c>
+      <c r="AG280" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH280" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM280" s="1" t="s">
         <v>1154</v>
-      </c>
-      <c r="AB280" s="1" t="s">
-        <v>1154</v>
-      </c>
-      <c r="AG280" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH280" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM280" s="1" t="s">
-        <v>1155</v>
       </c>
       <c r="AN280" s="1" t="n">
         <v>3</v>
@@ -22352,14 +22349,14 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B25" s="5" t="n">
         <f aca="false">MATCH(A25,$C$2:$C$207,0)</f>
         <v>24</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23048,26 +23045,26 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="B83" s="5" t="n">
         <f aca="false">MATCH(A83,$C$2:$C$207,0)</f>
         <v>82</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="5" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="B84" s="5" t="n">
         <f aca="false">MATCH(A84,$C$2:$C$207,0)</f>
         <v>83</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23132,14 +23129,14 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="5" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B90" s="5" t="n">
         <f aca="false">MATCH(A90,$C$2:$C$207,0)</f>
         <v>89</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23540,14 +23537,14 @@
     </row>
     <row r="124" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="5" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B124" s="5" t="n">
         <f aca="false">MATCH(A124,$C$2:$C$207,0)</f>
         <v>123</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23828,14 +23825,14 @@
     </row>
     <row r="148" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="5" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B148" s="5" t="n">
         <f aca="false">MATCH(A148,$C$2:$C$207,0)</f>
         <v>147</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23876,14 +23873,14 @@
     </row>
     <row r="152" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B152" s="5" t="n">
         <f aca="false">MATCH(A152,$C$2:$C$207,0)</f>
         <v>151</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23900,14 +23897,14 @@
     </row>
     <row r="154" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="5" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B154" s="5" t="n">
         <f aca="false">MATCH(A154,$C$2:$C$207,0)</f>
         <v>153</v>
       </c>
       <c r="C154" s="6" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23924,7 +23921,7 @@
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="5" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B156" s="5" t="e">
         <f aca="false">MATCH(A156,$C$2:$C$207,0)</f>
@@ -24032,7 +24029,7 @@
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="5" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="B165" s="5" t="e">
         <f aca="false">MATCH(A165,$C$2:$C$207,0)</f>
@@ -24044,7 +24041,7 @@
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="5" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B166" s="5" t="e">
         <f aca="false">MATCH(A166,$C$2:$C$207,0)</f>
@@ -24068,7 +24065,7 @@
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="5" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="B168" s="5" t="e">
         <f aca="false">MATCH(A168,$C$2:$C$207,0)</f>
@@ -24104,7 +24101,7 @@
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="5" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B171" s="5" t="e">
         <f aca="false">MATCH(A171,$C$2:$C$207,0)</f>

</xml_diff>